<commit_message>
add login and add_user test data, testcase and result
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="add_user" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>username</t>
   </si>
@@ -23,16 +23,91 @@
     <t>valid</t>
   </si>
   <si>
+    <t>testcase name</t>
+  </si>
+  <si>
     <t>student</t>
   </si>
   <si>
     <t>moodle</t>
   </si>
   <si>
+    <t>Valid testcase</t>
+  </si>
+  <si>
     <t>moodle123</t>
   </si>
   <si>
+    <t>Wrong password</t>
+  </si>
+  <si>
     <t>student123</t>
+  </si>
+  <si>
+    <t>Non exist username</t>
+  </si>
+  <si>
+    <t>Both field invalid</t>
+  </si>
+  <si>
+    <t>Empty password</t>
+  </si>
+  <si>
+    <t>Empty username</t>
+  </si>
+  <si>
+    <t>Both field empty</t>
+  </si>
+  <si>
+    <t>new_password</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>Bao</t>
+  </si>
+  <si>
+    <t>Tran</t>
+  </si>
+  <si>
+    <t>bao@gmail.com</t>
+  </si>
+  <si>
+    <t>Invalid first name</t>
+  </si>
+  <si>
+    <t>tester1</t>
+  </si>
+  <si>
+    <t>bao1@gmail.com</t>
+  </si>
+  <si>
+    <t>Invalid last name</t>
+  </si>
+  <si>
+    <t>admin@school.a</t>
+  </si>
+  <si>
+    <t>Invalid email</t>
+  </si>
+  <si>
+    <t>Invalid password</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>Invalid username</t>
   </si>
 </sst>
 </file>
@@ -303,70 +378,94 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="C8" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -383,7 +482,160 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.23456789E8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.23456789E8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.23456789E8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.23456789E8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.23456789E8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>